<commit_message>
Save all images and changes to Jupyter nbks
</commit_message>
<xml_diff>
--- a/GW_Plotting/output/check_counts.xlsx
+++ b/GW_Plotting/output/check_counts.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="180">
   <si>
     <t>country</t>
   </si>
@@ -193,6 +193,9 @@
     <t>FINLAND</t>
   </si>
   <si>
+    <t>FRANCE</t>
+  </si>
+  <si>
     <t>FRENCH GUIANA</t>
   </si>
   <si>
@@ -265,6 +268,9 @@
     <t>ISRAEL</t>
   </si>
   <si>
+    <t>ITALY</t>
+  </si>
+  <si>
     <t>JAMAICA</t>
   </si>
   <si>
@@ -527,6 +533,9 @@
   </si>
   <si>
     <t>UNITED KINGDOM</t>
+  </si>
+  <si>
+    <t>UNITED STATES</t>
   </si>
   <si>
     <t>URUGUAY</t>
@@ -902,7 +911,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B176"/>
+  <dimension ref="A1:B179"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1377,7 +1386,7 @@
         <v>59</v>
       </c>
       <c r="B59">
-        <v>63</v>
+        <v>205</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1385,7 +1394,7 @@
         <v>60</v>
       </c>
       <c r="B60">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1393,7 +1402,7 @@
         <v>61</v>
       </c>
       <c r="B61">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1401,7 +1410,7 @@
         <v>62</v>
       </c>
       <c r="B62">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1409,7 +1418,7 @@
         <v>63</v>
       </c>
       <c r="B63">
-        <v>21</v>
+        <v>63</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1417,7 +1426,7 @@
         <v>64</v>
       </c>
       <c r="B64">
-        <v>177</v>
+        <v>21</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1425,7 +1434,7 @@
         <v>65</v>
       </c>
       <c r="B65">
-        <v>63</v>
+        <v>177</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1433,7 +1442,7 @@
         <v>66</v>
       </c>
       <c r="B66">
-        <v>132</v>
+        <v>63</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1441,7 +1450,7 @@
         <v>67</v>
       </c>
       <c r="B67">
-        <v>63</v>
+        <v>132</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1465,7 +1474,7 @@
         <v>70</v>
       </c>
       <c r="B70">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1473,7 +1482,7 @@
         <v>71</v>
       </c>
       <c r="B71">
-        <v>55</v>
+        <v>72</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1481,7 +1490,7 @@
         <v>72</v>
       </c>
       <c r="B72">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1513,7 +1522,7 @@
         <v>76</v>
       </c>
       <c r="B76">
-        <v>183</v>
+        <v>63</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1521,7 +1530,7 @@
         <v>77</v>
       </c>
       <c r="B77">
-        <v>74</v>
+        <v>183</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1529,7 +1538,7 @@
         <v>78</v>
       </c>
       <c r="B78">
-        <v>142</v>
+        <v>74</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1537,7 +1546,7 @@
         <v>79</v>
       </c>
       <c r="B79">
-        <v>124</v>
+        <v>142</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1545,7 +1554,7 @@
         <v>80</v>
       </c>
       <c r="B80">
-        <v>89</v>
+        <v>124</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1553,7 +1562,7 @@
         <v>81</v>
       </c>
       <c r="B81">
-        <v>102</v>
+        <v>89</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1561,7 +1570,7 @@
         <v>82</v>
       </c>
       <c r="B82">
-        <v>83</v>
+        <v>102</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1569,7 +1578,7 @@
         <v>83</v>
       </c>
       <c r="B83">
-        <v>63</v>
+        <v>83</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1577,7 +1586,7 @@
         <v>84</v>
       </c>
       <c r="B84">
-        <v>63</v>
+        <v>153</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1593,7 +1602,7 @@
         <v>86</v>
       </c>
       <c r="B86">
-        <v>21</v>
+        <v>63</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1609,7 +1618,7 @@
         <v>88</v>
       </c>
       <c r="B88">
-        <v>52</v>
+        <v>21</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1617,7 +1626,7 @@
         <v>89</v>
       </c>
       <c r="B89">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1625,7 +1634,7 @@
         <v>90</v>
       </c>
       <c r="B90">
-        <v>21</v>
+        <v>52</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1633,7 +1642,7 @@
         <v>91</v>
       </c>
       <c r="B91">
-        <v>33</v>
+        <v>67</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1641,7 +1650,7 @@
         <v>92</v>
       </c>
       <c r="B92">
-        <v>81</v>
+        <v>21</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1649,7 +1658,7 @@
         <v>93</v>
       </c>
       <c r="B93">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1657,7 +1666,7 @@
         <v>94</v>
       </c>
       <c r="B94">
-        <v>63</v>
+        <v>81</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1665,7 +1674,7 @@
         <v>95</v>
       </c>
       <c r="B95">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1673,7 +1682,7 @@
         <v>96</v>
       </c>
       <c r="B96">
-        <v>21</v>
+        <v>63</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1681,7 +1690,7 @@
         <v>97</v>
       </c>
       <c r="B97">
-        <v>68</v>
+        <v>6</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1697,7 +1706,7 @@
         <v>99</v>
       </c>
       <c r="B99">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1705,7 +1714,7 @@
         <v>100</v>
       </c>
       <c r="B100">
-        <v>49</v>
+        <v>21</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1713,7 +1722,7 @@
         <v>101</v>
       </c>
       <c r="B101">
-        <v>43</v>
+        <v>70</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1721,7 +1730,7 @@
         <v>102</v>
       </c>
       <c r="B102">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1729,7 +1738,7 @@
         <v>103</v>
       </c>
       <c r="B103">
-        <v>63</v>
+        <v>43</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1737,7 +1746,7 @@
         <v>104</v>
       </c>
       <c r="B104">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -1745,7 +1754,7 @@
         <v>105</v>
       </c>
       <c r="B105">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -1761,7 +1770,7 @@
         <v>107</v>
       </c>
       <c r="B107">
-        <v>122</v>
+        <v>54</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1777,7 +1786,7 @@
         <v>109</v>
       </c>
       <c r="B109">
-        <v>7</v>
+        <v>122</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -1785,7 +1794,7 @@
         <v>110</v>
       </c>
       <c r="B110">
-        <v>51</v>
+        <v>63</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -1793,7 +1802,7 @@
         <v>111</v>
       </c>
       <c r="B111">
-        <v>85</v>
+        <v>7</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -1801,7 +1810,7 @@
         <v>112</v>
       </c>
       <c r="B112">
-        <v>86</v>
+        <v>51</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -1809,7 +1818,7 @@
         <v>113</v>
       </c>
       <c r="B113">
-        <v>22</v>
+        <v>85</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -1817,7 +1826,7 @@
         <v>114</v>
       </c>
       <c r="B114">
-        <v>63</v>
+        <v>86</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -1825,7 +1834,7 @@
         <v>115</v>
       </c>
       <c r="B115">
-        <v>167</v>
+        <v>22</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -1841,7 +1850,7 @@
         <v>117</v>
       </c>
       <c r="B117">
-        <v>135</v>
+        <v>167</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -1849,7 +1858,7 @@
         <v>118</v>
       </c>
       <c r="B118">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -1857,7 +1866,7 @@
         <v>119</v>
       </c>
       <c r="B119">
-        <v>55</v>
+        <v>135</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -1865,7 +1874,7 @@
         <v>120</v>
       </c>
       <c r="B120">
-        <v>98</v>
+        <v>71</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -1873,7 +1882,7 @@
         <v>121</v>
       </c>
       <c r="B121">
-        <v>43</v>
+        <v>55</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -1881,7 +1890,7 @@
         <v>122</v>
       </c>
       <c r="B122">
-        <v>181</v>
+        <v>98</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -1889,7 +1898,7 @@
         <v>123</v>
       </c>
       <c r="B123">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -1897,7 +1906,7 @@
         <v>124</v>
       </c>
       <c r="B124">
-        <v>41</v>
+        <v>181</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -1905,7 +1914,7 @@
         <v>125</v>
       </c>
       <c r="B125">
-        <v>21</v>
+        <v>49</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -1913,7 +1922,7 @@
         <v>126</v>
       </c>
       <c r="B126">
-        <v>65</v>
+        <v>41</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -1921,7 +1930,7 @@
         <v>127</v>
       </c>
       <c r="B127">
-        <v>63</v>
+        <v>21</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -1929,7 +1938,7 @@
         <v>128</v>
       </c>
       <c r="B128">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -1937,7 +1946,7 @@
         <v>129</v>
       </c>
       <c r="B129">
-        <v>126</v>
+        <v>63</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -1945,7 +1954,7 @@
         <v>130</v>
       </c>
       <c r="B130">
-        <v>103</v>
+        <v>63</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -1953,7 +1962,7 @@
         <v>131</v>
       </c>
       <c r="B131">
-        <v>213</v>
+        <v>126</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -1961,7 +1970,7 @@
         <v>132</v>
       </c>
       <c r="B132">
-        <v>143</v>
+        <v>103</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -1969,7 +1978,7 @@
         <v>133</v>
       </c>
       <c r="B133">
-        <v>1</v>
+        <v>213</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -1977,7 +1986,7 @@
         <v>134</v>
       </c>
       <c r="B134">
-        <v>64</v>
+        <v>143</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -1985,7 +1994,7 @@
         <v>135</v>
       </c>
       <c r="B135">
-        <v>63</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -1993,7 +2002,7 @@
         <v>136</v>
       </c>
       <c r="B136">
-        <v>156</v>
+        <v>64</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -2001,7 +2010,7 @@
         <v>137</v>
       </c>
       <c r="B137">
-        <v>51</v>
+        <v>63</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -2009,7 +2018,7 @@
         <v>138</v>
       </c>
       <c r="B138">
-        <v>63</v>
+        <v>156</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -2017,7 +2026,7 @@
         <v>139</v>
       </c>
       <c r="B139">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -2025,7 +2034,7 @@
         <v>140</v>
       </c>
       <c r="B140">
-        <v>78</v>
+        <v>63</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -2033,7 +2042,7 @@
         <v>141</v>
       </c>
       <c r="B141">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -2041,7 +2050,7 @@
         <v>142</v>
       </c>
       <c r="B142">
-        <v>7</v>
+        <v>78</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -2049,7 +2058,7 @@
         <v>143</v>
       </c>
       <c r="B143">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -2057,7 +2066,7 @@
         <v>144</v>
       </c>
       <c r="B144">
-        <v>63</v>
+        <v>7</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -2065,7 +2074,7 @@
         <v>145</v>
       </c>
       <c r="B145">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -2073,7 +2082,7 @@
         <v>146</v>
       </c>
       <c r="B146">
-        <v>21</v>
+        <v>63</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -2081,7 +2090,7 @@
         <v>147</v>
       </c>
       <c r="B147">
-        <v>21</v>
+        <v>56</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -2089,7 +2098,7 @@
         <v>148</v>
       </c>
       <c r="B148">
-        <v>61</v>
+        <v>21</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -2097,7 +2106,7 @@
         <v>149</v>
       </c>
       <c r="B149">
-        <v>63</v>
+        <v>21</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -2105,7 +2114,7 @@
         <v>150</v>
       </c>
       <c r="B150">
-        <v>129</v>
+        <v>61</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -2113,7 +2122,7 @@
         <v>151</v>
       </c>
       <c r="B151">
-        <v>183</v>
+        <v>63</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -2121,7 +2130,7 @@
         <v>152</v>
       </c>
       <c r="B152">
-        <v>63</v>
+        <v>129</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -2129,7 +2138,7 @@
         <v>153</v>
       </c>
       <c r="B153">
-        <v>62</v>
+        <v>183</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -2145,7 +2154,7 @@
         <v>155</v>
       </c>
       <c r="B155">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -2153,7 +2162,7 @@
         <v>156</v>
       </c>
       <c r="B156">
-        <v>175</v>
+        <v>63</v>
       </c>
     </row>
     <row r="157" spans="1:2">
@@ -2161,7 +2170,7 @@
         <v>157</v>
       </c>
       <c r="B157">
-        <v>155</v>
+        <v>61</v>
       </c>
     </row>
     <row r="158" spans="1:2">
@@ -2169,7 +2178,7 @@
         <v>158</v>
       </c>
       <c r="B158">
-        <v>117</v>
+        <v>175</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -2177,7 +2186,7 @@
         <v>159</v>
       </c>
       <c r="B159">
-        <v>21</v>
+        <v>155</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -2185,7 +2194,7 @@
         <v>160</v>
       </c>
       <c r="B160">
-        <v>79</v>
+        <v>117</v>
       </c>
     </row>
     <row r="161" spans="1:2">
@@ -2193,7 +2202,7 @@
         <v>161</v>
       </c>
       <c r="B161">
-        <v>63</v>
+        <v>21</v>
       </c>
     </row>
     <row r="162" spans="1:2">
@@ -2201,7 +2210,7 @@
         <v>162</v>
       </c>
       <c r="B162">
-        <v>63</v>
+        <v>79</v>
       </c>
     </row>
     <row r="163" spans="1:2">
@@ -2209,7 +2218,7 @@
         <v>163</v>
       </c>
       <c r="B163">
-        <v>105</v>
+        <v>63</v>
       </c>
     </row>
     <row r="164" spans="1:2">
@@ -2217,7 +2226,7 @@
         <v>164</v>
       </c>
       <c r="B164">
-        <v>89</v>
+        <v>63</v>
       </c>
     </row>
     <row r="165" spans="1:2">
@@ -2225,7 +2234,7 @@
         <v>165</v>
       </c>
       <c r="B165">
-        <v>148</v>
+        <v>105</v>
       </c>
     </row>
     <row r="166" spans="1:2">
@@ -2233,7 +2242,7 @@
         <v>166</v>
       </c>
       <c r="B166">
-        <v>21</v>
+        <v>89</v>
       </c>
     </row>
     <row r="167" spans="1:2">
@@ -2241,7 +2250,7 @@
         <v>167</v>
       </c>
       <c r="B167">
-        <v>63</v>
+        <v>148</v>
       </c>
     </row>
     <row r="168" spans="1:2">
@@ -2257,7 +2266,7 @@
         <v>169</v>
       </c>
       <c r="B169">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="170" spans="1:2">
@@ -2265,7 +2274,7 @@
         <v>170</v>
       </c>
       <c r="B170">
-        <v>262</v>
+        <v>21</v>
       </c>
     </row>
     <row r="171" spans="1:2">
@@ -2273,7 +2282,7 @@
         <v>171</v>
       </c>
       <c r="B171">
-        <v>81</v>
+        <v>54</v>
       </c>
     </row>
     <row r="172" spans="1:2">
@@ -2281,7 +2290,7 @@
         <v>172</v>
       </c>
       <c r="B172">
-        <v>21</v>
+        <v>262</v>
       </c>
     </row>
     <row r="173" spans="1:2">
@@ -2289,7 +2298,7 @@
         <v>173</v>
       </c>
       <c r="B173">
-        <v>102</v>
+        <v>202</v>
       </c>
     </row>
     <row r="174" spans="1:2">
@@ -2297,7 +2306,7 @@
         <v>174</v>
       </c>
       <c r="B174">
-        <v>22</v>
+        <v>81</v>
       </c>
     </row>
     <row r="175" spans="1:2">
@@ -2305,7 +2314,7 @@
         <v>175</v>
       </c>
       <c r="B175">
-        <v>49</v>
+        <v>21</v>
       </c>
     </row>
     <row r="176" spans="1:2">
@@ -2313,6 +2322,30 @@
         <v>176</v>
       </c>
       <c r="B176">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2">
+      <c r="A177" t="s">
+        <v>177</v>
+      </c>
+      <c r="B177">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2">
+      <c r="A178" t="s">
+        <v>178</v>
+      </c>
+      <c r="B178">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2">
+      <c r="A179" t="s">
+        <v>179</v>
+      </c>
+      <c r="B179">
         <v>96</v>
       </c>
     </row>

</xml_diff>